<commit_message>
How to read an uploaded file
</commit_message>
<xml_diff>
--- a/src/EPPlus.Core.SampleWebApp/wwwroot/reports/report.xlsx
+++ b/src/EPPlus.Core.SampleWebApp/wwwroot/reports/report.xlsx
@@ -187,9 +187,12 @@
       </c>
     </row>
   </sheetData>
-  <headerFooter/>
+  <headerFooter>
+    <oddFooter>&amp;R&amp;G</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>